<commit_message>
Modified: Export to excel
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>port</t>
-  </si>
-  <si>
-    <t>status</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>My_Viettel</t>
@@ -369,19 +369,19 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>3000</v>
       </c>
-      <c r="B2" t="b">
+      <c r="E2" t="b">
         <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Update to import excel
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -41,13 +41,31 @@
   </si>
   <si>
     <t>192.168.1.0</t>
+  </si>
+  <si>
+    <t>Viettel_Digital</t>
+  </si>
+  <si>
+    <t>192.168.1.12</t>
+  </si>
+  <si>
+    <t>Viettel_CyberSpace</t>
+  </si>
+  <si>
+    <t>10.10.1.2</t>
+  </si>
+  <si>
+    <t>Viettel_Money</t>
+  </si>
+  <si>
+    <t>10.10.1.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,7 +100,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -339,18 +365,31 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -367,7 +406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -384,7 +423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -401,6 +440,58 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>